<commit_message>
changement calculs capteur bord + modif bom
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -1,26 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paul_\OneDrive\Bureau\ESE\ProjetRobot\2425_ESE_Projet_Torero\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeanp\Documents\ENSEA\3A\PROJET\2425_ESE_Projet_Torero\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A33AADB3-DBEF-4947-9E1E-F3C238FE2365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D219D73E-7E7F-47AE-9061-56A76C4EC26F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
   <si>
     <t xml:space="preserve">REFERENCE </t>
   </si>
@@ -134,6 +145,9 @@
   </si>
   <si>
     <t>1467857/1467858</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Résistance boot flash user button </t>
   </si>
 </sst>
 </file>
@@ -158,7 +172,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -168,6 +182,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA6A6A6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -205,7 +225,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -215,12 +235,6 @@
     </xf>
     <xf numFmtId="4" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -233,6 +247,17 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="3" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -541,24 +566,24 @@
   <dimension ref="A1:J43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="B1" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.26953125" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.26953125" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.26953125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -580,7 +605,7 @@
       <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="6" t="s">
         <v>6</v>
       </c>
       <c r="I1" s="1" t="s">
@@ -590,25 +615,25 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2">
+    <row r="2" spans="1:10" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9">
         <v>1</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" t="s">
+      <c r="B2" s="10"/>
+      <c r="C2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="5"/>
-      <c r="H2" s="9">
+      <c r="G2" s="11"/>
+      <c r="H2" s="12">
         <f t="shared" ref="H2:H15" si="0">B2*G2</f>
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3">
+    <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="9">
         <v>2</v>
       </c>
       <c r="C3" t="s">
@@ -620,13 +645,13 @@
       <c r="F3" t="s">
         <v>32</v>
       </c>
-      <c r="H3" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4">
+      <c r="H3" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="9">
         <v>3</v>
       </c>
       <c r="C4" t="s">
@@ -638,13 +663,13 @@
       <c r="F4" t="s">
         <v>32</v>
       </c>
-      <c r="H4" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5">
+      <c r="H4" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="9">
         <v>4</v>
       </c>
       <c r="C5" t="s">
@@ -653,13 +678,13 @@
       <c r="D5" t="s">
         <v>25</v>
       </c>
-      <c r="H5" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6">
+      <c r="H5" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
         <v>5</v>
       </c>
       <c r="C6" t="s">
@@ -668,13 +693,13 @@
       <c r="D6" t="s">
         <v>23</v>
       </c>
-      <c r="H6" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7">
+      <c r="H6" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
         <v>6</v>
       </c>
       <c r="C7" t="s">
@@ -683,13 +708,13 @@
       <c r="D7" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8">
+      <c r="H7" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
         <v>7</v>
       </c>
       <c r="C8" t="s">
@@ -698,13 +723,13 @@
       <c r="D8" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9">
+      <c r="H8" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="9">
         <v>8</v>
       </c>
       <c r="C9" t="s">
@@ -713,13 +738,13 @@
       <c r="D9" t="s">
         <v>19</v>
       </c>
-      <c r="H9" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10">
+      <c r="H9" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
         <v>9</v>
       </c>
       <c r="C10" t="s">
@@ -728,16 +753,16 @@
       <c r="D10" t="s">
         <v>28</v>
       </c>
-      <c r="H10" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11">
+      <c r="H10" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="9">
         <v>10</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="4">
         <v>2</v>
       </c>
       <c r="C11" t="s">
@@ -752,13 +777,13 @@
       <c r="F11" t="s">
         <v>32</v>
       </c>
-      <c r="H11" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12">
+      <c r="H11" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="9">
         <v>11</v>
       </c>
       <c r="C12" t="s">
@@ -767,31 +792,31 @@
       <c r="D12" t="s">
         <v>31</v>
       </c>
-      <c r="H12" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13">
+      <c r="H12" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="9">
         <v>12</v>
       </c>
       <c r="C13" t="s">
         <v>12</v>
       </c>
-      <c r="H13" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14">
+      <c r="H13" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="9">
         <v>13</v>
       </c>
       <c r="C14" t="s">
         <v>14</v>
       </c>
-      <c r="H14" s="9">
+      <c r="H14" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -799,11 +824,11 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="4">
         <v>2</v>
       </c>
       <c r="C15" t="s">
@@ -818,150 +843,157 @@
       <c r="F15" t="s">
         <v>32</v>
       </c>
-      <c r="G15" s="7">
+      <c r="G15" s="5">
         <v>0.37</v>
       </c>
-      <c r="H15" s="9">
+      <c r="H15" s="7">
         <f t="shared" si="0"/>
         <v>0.74</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I15" s="13"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B16" s="4">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>

</xml_diff>